<commit_message>
Added new client write functionality
</commit_message>
<xml_diff>
--- a/RoSATron/ExcelData/Clients.xlsx
+++ b/RoSATron/ExcelData/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Embrey_J_Krasner_A-P0\RoSATron\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292F2026-CC0E-4957-A21E-896F4FF3642E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7941D8F-904D-4CC8-B32C-F4D678EF15BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DC2EA3-C148-42E5-9646-070198748FCC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -498,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0026A6E-D28A-4737-9C9E-9F29273C5BC1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>